<commit_message>
Changes in the xml and xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UIVML\Downloads\Documentación UIVML\Cooperaciones internacionales\Cooperación SIM\CABUREK\XML DCC\De excel a xml en python\lxml\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ME-02\OneDrive\Documentos\Plan CABUREK\XML DCC\De excel a xml en python\lxml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ECC61F-899F-4FCE-B859-1DB6F9D4D006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="2940" windowWidth="20295" windowHeight="5355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="195" yWindow="2940" windowWidth="20295" windowHeight="5355"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,44 +37,226 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>ME-02</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ME-02:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+No.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>basic_referenceValue</t>
-  </si>
-  <si>
-    <t>basic_measuredValue</t>
-  </si>
-  <si>
-    <t>basic_measurementError</t>
-  </si>
-  <si>
-    <t>uncertainty</t>
-  </si>
-  <si>
-    <t>distribution</t>
-  </si>
-  <si>
-    <t>k_factor</t>
-  </si>
-  <si>
-    <t>coverageProb</t>
-  </si>
-  <si>
-    <t>ds18b20_id</t>
-  </si>
-  <si>
-    <t>vertical</t>
-  </si>
-  <si>
-    <t>Casio</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Modificación o Reposición</t>
+  </si>
+  <si>
+    <t>Instrumento</t>
+  </si>
+  <si>
+    <t>Fabricante</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>No. de serie</t>
+  </si>
+  <si>
+    <t>No. de identificación interna</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>No. de registro</t>
+  </si>
+  <si>
+    <t>Hojas de este certificado</t>
+  </si>
+  <si>
+    <t>Fecha de recepción</t>
+  </si>
+  <si>
+    <t>Fecha de calibración</t>
+  </si>
+  <si>
+    <t>Fecha de emisión de certificado</t>
+  </si>
+  <si>
+    <t>Calibró</t>
+  </si>
+  <si>
+    <t>Autorizó</t>
+  </si>
+  <si>
+    <t>Presión atmosférica</t>
+  </si>
+  <si>
+    <t>Variación de presión</t>
+  </si>
+  <si>
+    <t>Temperatura</t>
+  </si>
+  <si>
+    <t>Variación de temperatura</t>
+  </si>
+  <si>
+    <t>Humedad Relativa</t>
+  </si>
+  <si>
+    <t>Variación de humedad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo de termómetro </t>
+  </si>
+  <si>
+    <t>Marca</t>
+  </si>
+  <si>
+    <t>Modelo</t>
+  </si>
+  <si>
+    <t>Intervalo de indicación</t>
+  </si>
+  <si>
+    <t>División de escala</t>
+  </si>
+  <si>
+    <t>Indicador de profundidad de Inmersión</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>CONDICIÓN, aplica</t>
+  </si>
+  <si>
+    <t>Condición</t>
+  </si>
+  <si>
+    <t>Método de calibración</t>
+  </si>
+  <si>
+    <t>El método utilizado por el CENAME tuvo alguna adición, desviación o exclusión al realizar la calibración del instrumento:</t>
+  </si>
+  <si>
+    <t>Describa:</t>
+  </si>
+  <si>
+    <t>Patrones y equipo utilizados</t>
+  </si>
+  <si>
+    <t>Temperatura °C</t>
+  </si>
+  <si>
+    <t>Corrección °C</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Incertidumbre Expandida </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± °C</t>
+    </r>
+  </si>
+  <si>
+    <t>Temperatura °F</t>
+  </si>
+  <si>
+    <t>Corrección °F</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Incertidumbre Expandida </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± °F</t>
+    </r>
+  </si>
+  <si>
+    <t>DECLARACIÓN DE LA CONFORMIDAD (de ser aplicable)</t>
+  </si>
+  <si>
+    <t>Describa Regla de Decisión</t>
+  </si>
+  <si>
+    <t>OPINIONES/INTERPRETACIONES TÉCNICAS (de ser aplicable)</t>
+  </si>
+  <si>
+    <t>Opiniones/Interpretaciones Técnicas</t>
+  </si>
+  <si>
+    <t>Declaración de la conformidad</t>
+  </si>
+  <si>
+    <t>Opiniones/interpretaciones técnicas</t>
+  </si>
+  <si>
+    <t>TE-001</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Adición</t>
+  </si>
+  <si>
+    <t>Desviación</t>
+  </si>
+  <si>
+    <t>Exclusión al método</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +269,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -107,8 +310,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -124,6 +335,150 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="REGISTROS"/>
+      <sheetName val="CALCULOS"/>
+      <sheetName val="EST INCERTI"/>
+      <sheetName val="RESULTADOS"/>
+      <sheetName val="DCC"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3">
+        <row r="12">
+          <cell r="C12">
+            <v>1.1100000000000001</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="C16" t="str">
+            <v>Baño ISOTECH 796 M</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="C20">
+            <v>21.375</v>
+          </cell>
+          <cell r="D20">
+            <v>0.80000000000000071</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="C21">
+            <v>57.637500000000003</v>
+          </cell>
+          <cell r="D21">
+            <v>1.5500000000000007</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="C22">
+            <v>852.26249999999993</v>
+          </cell>
+          <cell r="D22">
+            <v>1.3999999999999773</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26">
+            <v>-18</v>
+          </cell>
+          <cell r="C26">
+            <v>1.455711007999998</v>
+          </cell>
+          <cell r="D26">
+            <v>0.32378336378922667</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27">
+            <v>4</v>
+          </cell>
+          <cell r="C27">
+            <v>1.2475292799999993</v>
+          </cell>
+          <cell r="D27">
+            <v>0.32316507649600179</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28">
+            <v>65</v>
+          </cell>
+          <cell r="C28">
+            <v>1.1083083899999977</v>
+          </cell>
+          <cell r="D28">
+            <v>0.32830727476963817</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="B29">
+            <v>90</v>
+          </cell>
+          <cell r="C29">
+            <v>0.57803948000000105</v>
+          </cell>
+          <cell r="D29">
+            <v>0.32830727476963817</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="B32">
+            <v>-0.39999999999999858</v>
+          </cell>
+          <cell r="C32">
+            <v>2.6202798143999928</v>
+          </cell>
+          <cell r="D32">
+            <v>0.58281005482060522</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="B33">
+            <v>39.200000000000003</v>
+          </cell>
+          <cell r="C33">
+            <v>2.2455527039999978</v>
+          </cell>
+          <cell r="D33">
+            <v>0.58169713769280662</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="B34">
+            <v>149</v>
+          </cell>
+          <cell r="C34">
+            <v>1.9949551019999987</v>
+          </cell>
+          <cell r="D34">
+            <v>0.59095309458535183</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="B35">
+            <v>194</v>
+          </cell>
+          <cell r="C35">
+            <v>1.0404710640000019</v>
+          </cell>
+          <cell r="D35">
+            <v>0.59095309458535183</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -388,14 +743,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AV6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
@@ -407,71 +760,374 @@
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
+    <row r="1" spans="1:48" ht="270" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2">
+        <f>[1]REGISTROS!C7</f>
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="F2" s="2">
+        <f>[1]REGISTROS!C8</f>
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="H2">
+        <f>[1]REGISTROS!C2</f>
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>1E-4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>95</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
+      <c r="K2">
+        <f>[1]REGISTROS!H2</f>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f>[1]REGISTROS!I23</f>
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <f>[1]RESULTADOS!C22</f>
+        <v>852.26249999999993</v>
+      </c>
+      <c r="Q2">
+        <f>[1]RESULTADOS!D22</f>
+        <v>1.3999999999999773</v>
+      </c>
+      <c r="R2">
+        <f>[1]RESULTADOS!C20</f>
+        <v>21.375</v>
+      </c>
+      <c r="S2">
+        <f>[1]RESULTADOS!D20</f>
+        <v>0.80000000000000071</v>
+      </c>
+      <c r="T2">
+        <f>[1]RESULTADOS!C21</f>
+        <v>57.637500000000003</v>
+      </c>
+      <c r="U2">
+        <f>[1]RESULTADOS!D21</f>
+        <v>1.5500000000000007</v>
+      </c>
+      <c r="W2">
+        <f>[1]REGISTROS!C6</f>
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <f>[1]REGISTROS!C7</f>
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <f>[1]RESULTADOS!C12</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="AH2" t="str">
+        <f>[1]RESULTADOS!C16</f>
+        <v>Baño ISOTECH 796 M</v>
+      </c>
+      <c r="AI2" s="3">
+        <f>[1]RESULTADOS!B26</f>
+        <v>-18</v>
+      </c>
+      <c r="AJ2" s="3">
+        <f>[1]RESULTADOS!C26</f>
+        <v>1.455711007999998</v>
+      </c>
+      <c r="AK2" s="3">
+        <f>[1]RESULTADOS!D26</f>
+        <v>0.32378336378922667</v>
+      </c>
+      <c r="AL2" s="3">
+        <f>[1]RESULTADOS!B32</f>
+        <v>-0.39999999999999858</v>
+      </c>
+      <c r="AM2" s="3">
+        <f>[1]RESULTADOS!C32</f>
+        <v>2.6202798143999928</v>
+      </c>
+      <c r="AN2" s="3">
+        <f>[1]RESULTADOS!D32</f>
+        <v>0.58281005482060522</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AI3" s="3">
+        <f>[1]RESULTADOS!B27</f>
+        <v>4</v>
+      </c>
+      <c r="AJ3" s="3">
+        <f>[1]RESULTADOS!C27</f>
+        <v>1.2475292799999993</v>
+      </c>
+      <c r="AK3" s="3">
+        <f>[1]RESULTADOS!D27</f>
+        <v>0.32316507649600179</v>
+      </c>
+      <c r="AL3" s="3">
+        <f>[1]RESULTADOS!B33</f>
+        <v>39.200000000000003</v>
+      </c>
+      <c r="AM3" s="3">
+        <f>[1]RESULTADOS!C33</f>
+        <v>2.2455527039999978</v>
+      </c>
+      <c r="AN3" s="3">
+        <f>[1]RESULTADOS!D33</f>
+        <v>0.58169713769280662</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AI4" s="3">
+        <f>[1]RESULTADOS!B28</f>
+        <v>65</v>
+      </c>
+      <c r="AJ4" s="3">
+        <f>[1]RESULTADOS!C28</f>
+        <v>1.1083083899999977</v>
+      </c>
+      <c r="AK4" s="3">
+        <f>[1]RESULTADOS!D28</f>
+        <v>0.32830727476963817</v>
+      </c>
+      <c r="AL4" s="3">
+        <f>[1]RESULTADOS!B34</f>
+        <v>149</v>
+      </c>
+      <c r="AM4" s="3">
+        <f>[1]RESULTADOS!C34</f>
+        <v>1.9949551019999987</v>
+      </c>
+      <c r="AN4" s="3">
+        <f>[1]RESULTADOS!D34</f>
+        <v>0.59095309458535183</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AI5" s="3">
+        <f>[1]RESULTADOS!B29</f>
+        <v>90</v>
+      </c>
+      <c r="AJ5" s="3">
+        <f>[1]RESULTADOS!C29</f>
+        <v>0.57803948000000105</v>
+      </c>
+      <c r="AK5" s="3">
+        <f>[1]RESULTADOS!D29</f>
+        <v>0.32830727476963817</v>
+      </c>
+      <c r="AL5" s="3">
+        <f>[1]RESULTADOS!B35</f>
+        <v>194</v>
+      </c>
+      <c r="AM5" s="3">
+        <f>[1]RESULTADOS!C35</f>
+        <v>1.0404710640000019</v>
+      </c>
+      <c r="AN5" s="3">
+        <f>[1]RESULTADOS!D35</f>
+        <v>0.59095309458535183</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AT6" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2">
+      <formula1>$AV$2:$AV$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2">
+      <formula1>$AU$2:$AU$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2">
+      <formula1>$AT$2:$AT$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2">
+      <formula1>$AS$2:$AS$3</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>